<commit_message>
feat: updated search sugg sorting
</commit_message>
<xml_diff>
--- a/uploads/MDSD - Md. Delwar Shahadat Deepu.xlsx
+++ b/uploads/MDSD - Md. Delwar Shahadat Deepu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
   <si>
     <t>United International University</t>
   </si>
@@ -47,100 +47,115 @@
     <t>Room:</t>
   </si>
   <si>
+    <t>935(B)</t>
+  </si>
+  <si>
     <t>Email:</t>
   </si>
   <si>
+    <t>mdsdeepu3@gmail.com</t>
+  </si>
+  <si>
+    <t>Undergraduate Program</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>08:31 AM - 09:50 AM</t>
+  </si>
+  <si>
+    <t>09:51 AM - 11:10 AM</t>
+  </si>
+  <si>
+    <t>11:11 AM - 12:30 PM</t>
+  </si>
+  <si>
+    <t>12:31 PM - 01:50 PM</t>
+  </si>
+  <si>
+    <t>01:51 PM - 03:10 PM</t>
+  </si>
+  <si>
+    <t>03:11 PM - 04:30 PM</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>CSE 1326 (L): 508</t>
+  </si>
+  <si>
+    <t>CSE 1326 (O): 825</t>
+  </si>
+  <si>
+    <t>CnH</t>
+  </si>
+  <si>
+    <t>SUN</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>CSE 3712 (B): 424</t>
+  </si>
+  <si>
+    <t>TUE</t>
+  </si>
+  <si>
+    <t>CSE 1110 (M): 326</t>
+  </si>
+  <si>
+    <t>CSE 1110 (H): 326</t>
+  </si>
+  <si>
+    <t>WED</t>
+  </si>
+  <si>
+    <t>Graduate Program</t>
+  </si>
+  <si>
+    <t>08:00 AM - 10:30 PM / 08:30 AM - 11:00 AM</t>
+  </si>
+  <si>
+    <t>10:30 AM - 01:00 PM / 11:00 AM - 01:30 PM</t>
+  </si>
+  <si>
+    <t>02:30 PM - 05:00 PM</t>
+  </si>
+  <si>
+    <t>FRI</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Class Hour:</t>
+  </si>
+  <si>
+    <t>Counselling Hour:</t>
+  </si>
+  <si>
+    <t>Office Hour:</t>
+  </si>
+  <si>
+    <t>Total Weekly Hours:</t>
+  </si>
+  <si>
+    <t>Signature of the Faculty Member</t>
+  </si>
+  <si>
+    <t>Head/Director's Signature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: </t>
+  </si>
+  <si>
     <t>mdeepu202037@bscse.uiu.ac.bd</t>
-  </si>
-  <si>
-    <t>Undergraduate Program</t>
-  </si>
-  <si>
-    <t>DAY</t>
-  </si>
-  <si>
-    <t>08:31 AM - 09:50 AM</t>
-  </si>
-  <si>
-    <t>09:51 AM - 11:10 AM</t>
-  </si>
-  <si>
-    <t>11:11 AM - 12:30 PM</t>
-  </si>
-  <si>
-    <t>12:31 PM - 01:50 PM</t>
-  </si>
-  <si>
-    <t>01:51 PM - 03:10 PM</t>
-  </si>
-  <si>
-    <t>03:11 PM - 04:30 PM</t>
-  </si>
-  <si>
-    <t>SAT</t>
-  </si>
-  <si>
-    <t>CSE 1326 (L): 508</t>
-  </si>
-  <si>
-    <t>CSE 1326 (O): 825</t>
-  </si>
-  <si>
-    <t>SUN</t>
-  </si>
-  <si>
-    <t>MON</t>
-  </si>
-  <si>
-    <t>CSE 3712 (B): 424</t>
-  </si>
-  <si>
-    <t>TUE</t>
-  </si>
-  <si>
-    <t>CSE 1110 (M): 326</t>
-  </si>
-  <si>
-    <t>CSE 1110 (H): 326</t>
-  </si>
-  <si>
-    <t>WED</t>
-  </si>
-  <si>
-    <t>Graduate Program</t>
-  </si>
-  <si>
-    <t>08:00 AM - 10:30 PM / 08:30 AM - 11:00 AM</t>
-  </si>
-  <si>
-    <t>10:30 AM - 01:00 PM / 11:00 AM - 01:30 PM</t>
-  </si>
-  <si>
-    <t>02:30 PM - 05:00 PM</t>
-  </si>
-  <si>
-    <t>FRI</t>
-  </si>
-  <si>
-    <t>Class Hour:</t>
-  </si>
-  <si>
-    <t>Counselling Hour:</t>
-  </si>
-  <si>
-    <t>Office Hour:</t>
-  </si>
-  <si>
-    <t>Total Weekly Hours:</t>
-  </si>
-  <si>
-    <t>Signature of the Faculty Member</t>
-  </si>
-  <si>
-    <t>Head/Director's Signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date: </t>
   </si>
 </sst>
 </file>
@@ -229,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -239,6 +254,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -251,6 +269,9 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,20 +579,22 @@
       <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
@@ -605,132 +628,158 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="6" t="s">
+      <c r="I13" s="8"/>
+      <c r="J13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="7"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="7"/>
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="7"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
@@ -764,65 +813,77 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="7"/>
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="7"/>
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="7"/>
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
@@ -856,32 +917,32 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="10">
+        <v>40</v>
+      </c>
+      <c r="C27" s="12">
         <v>13.33</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="10">
+        <v>41</v>
+      </c>
+      <c r="F27" s="12">
         <f>4/3 * COUNTIF($B$14:$M$18, "CnH*") + 2.5 * COUNTIF($B$23:$M$24, "CnH*")</f>
-        <v>0</v>
+        <v>13.33333333</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="10">
+        <v>42</v>
+      </c>
+      <c r="I27" s="12">
         <f>4/3 * COUNTIF($B$14:$M$18, "OH*") + 2.5 * COUNTIF($B$23:$M$24, "OH*")</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="J27" s="5"/>
       <c r="K27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="10">
+        <v>43</v>
+      </c>
+      <c r="M27" s="12">
         <f>C27+F27+I27</f>
-        <v>13.33</v>
+        <v>30.66333333</v>
       </c>
     </row>
     <row r="28">
@@ -944,23 +1005,23 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="s">
-        <v>40</v>
+      <c r="A33" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="11" t="s">
-        <v>41</v>
+      <c r="H33" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="s">
-        <v>42</v>
+      <c r="A34" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -968,8 +1029,8 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="11" t="s">
-        <v>42</v>
+      <c r="H34" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1140,20 +1201,20 @@
       <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
@@ -1187,132 +1248,132 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="6" t="s">
+      <c r="I13" s="8"/>
+      <c r="J13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="7"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="7"/>
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="7"/>
+      <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
@@ -1346,65 +1407,65 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="7"/>
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="7"/>
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="7"/>
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
@@ -1438,30 +1499,30 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="10">
+        <v>40</v>
+      </c>
+      <c r="C27" s="12">
         <v>13.33</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="10">
+        <v>41</v>
+      </c>
+      <c r="F27" s="12">
         <f>4/3 * COUNTIF($B$14:$M$18, "CnH*") + 2.5 * COUNTIF($B$23:$M$24, "CnH*")</f>
         <v>0</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="10">
+        <v>42</v>
+      </c>
+      <c r="I27" s="12">
         <f>4/3 * COUNTIF($B$14:$M$18, "OH*") + 2.5 * COUNTIF($B$23:$M$24, "OH*")</f>
         <v>0</v>
       </c>
-      <c r="J27" s="4"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="10">
+        <v>43</v>
+      </c>
+      <c r="M27" s="12">
         <f>C27+F27+I27</f>
         <v>13.33</v>
       </c>
@@ -1526,23 +1587,23 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="s">
-        <v>40</v>
+      <c r="A33" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="11" t="s">
-        <v>41</v>
+      <c r="H33" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="s">
-        <v>42</v>
+      <c r="A34" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1550,8 +1611,8 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="11" t="s">
-        <v>42</v>
+      <c r="H34" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>

</xml_diff>